<commit_message>
Cambios en la rama de pruebas
</commit_message>
<xml_diff>
--- a/Reporte_Alumnos_20241021.xlsx
+++ b/Reporte_Alumnos_20241021.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A8:L10"/>
+  <dimension ref="A8:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,59 +521,175 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Estrada</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Manuel</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>36526</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>MGGG910120MOCQCH82</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>albino garcia</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>zapata</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>adsad@aa.co</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>1234567865</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>RGVS 001 006 001</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>3</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Rosas</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Rojas</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Rosa</t>
         </is>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E11" s="1" t="n">
         <v>36893</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>FEMJ680914HTCAOK54</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Miguel Hidalgo</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>loma</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>11@d.d</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>1234560987</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>RGVS 001 006 000</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Yepez</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Lorenzo</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Emmanuel</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>45576</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>FAAA990318MGRRLR08</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>albino garcia2</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>loma</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>adsad@aa</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>1234560987</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>RGVS 001 006 002</t>
         </is>
       </c>
     </row>

</xml_diff>